<commit_message>
Hard code some parameters
Change some universal or "by-definition" parameters to be hard-coded
into the model
</commit_message>
<xml_diff>
--- a/autumn/xls/TB_generalepi_macro_constants.xlsx
+++ b/autumn/xls/TB_generalepi_macro_constants.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="549" uniqueCount="148">
   <si>
     <t>best</t>
   </si>
@@ -343,15 +343,6 @@
     <t>epi_proportion_cases_extrapul</t>
   </si>
   <si>
-    <t>tb_multiplier_force_smearpos</t>
-  </si>
-  <si>
-    <t>tb_multiplier_force_extrapul</t>
-  </si>
-  <si>
-    <t>tb_multiplier_force</t>
-  </si>
-  <si>
     <t>tb_n_contact</t>
   </si>
   <si>
@@ -437,9 +428,6 @@
   </si>
   <si>
     <t>program_prop_nonsuccessoutcomes_death</t>
-  </si>
-  <si>
-    <t>epi_proportion_cases</t>
   </si>
   <si>
     <t>tb_multiplier_force_smearneg</t>
@@ -50600,10 +50588,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -50618,10 +50606,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -50706,10 +50694,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="71" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C8" s="73">
-        <v>1</v>
+        <v>0.24</v>
       </c>
       <c r="D8" s="70"/>
       <c r="E8" s="70"/>
@@ -50719,64 +50707,64 @@
         <v>105</v>
       </c>
       <c r="C9" s="73">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="71" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C10" s="73">
-        <v>0.24</v>
+        <v>0.12</v>
       </c>
       <c r="D10" s="70"/>
       <c r="E10" s="70"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="71" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="C11" s="73">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C12" s="73">
-        <v>1</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D12" s="70"/>
       <c r="E12" s="70"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="71" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="C13" s="73">
-        <v>14</v>
+        <v>0.7</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="71" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C14" s="73">
-        <v>0.12</v>
+        <v>0.2</v>
       </c>
       <c r="D14" s="70"/>
       <c r="E14" s="70"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="71" t="s">
-        <v>140</v>
+        <v>107</v>
       </c>
       <c r="C15" s="73">
         <v>0.4</v>
@@ -50786,81 +50774,81 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="71" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C16" s="73">
-        <v>7.0000000000000001E-3</v>
+        <v>3</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="70"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="71" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C17" s="73">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="71" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C18" s="73">
-        <v>0.2</v>
+        <v>0.88</v>
       </c>
       <c r="D18" s="70"/>
       <c r="E18" s="70"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="71" t="s">
-        <v>110</v>
+        <v>141</v>
       </c>
       <c r="C19" s="73">
-        <v>0.4</v>
+        <f>1-C18</f>
+        <v>0.12</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="70"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="71" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C20" s="73">
-        <v>3</v>
+        <v>0.8</v>
       </c>
       <c r="D20" s="70"/>
       <c r="E20" s="70"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="71" t="s">
-        <v>143</v>
+        <v>110</v>
       </c>
       <c r="C21" s="73">
-        <v>0.5</v>
+        <v>0.9</v>
       </c>
       <c r="D21" s="70"/>
       <c r="E21" s="70"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="71" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C22" s="73">
-        <v>0.88</v>
+        <v>26</v>
       </c>
       <c r="D22" s="70"/>
       <c r="E22" s="70"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="71" t="s">
-        <v>145</v>
+        <v>111</v>
       </c>
       <c r="C23" s="73">
-        <f>1-C22</f>
-        <v>0.12</v>
+        <v>0.5</v>
       </c>
       <c r="D23" s="70"/>
       <c r="E23" s="70"/>
@@ -50870,7 +50858,7 @@
         <v>112</v>
       </c>
       <c r="C24" s="73">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="D24" s="70"/>
       <c r="E24" s="70"/>
@@ -50880,27 +50868,27 @@
         <v>113</v>
       </c>
       <c r="C25" s="73">
-        <v>0.9</v>
+        <v>3</v>
       </c>
       <c r="D25" s="70"/>
       <c r="E25" s="70"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="71" t="s">
-        <v>146</v>
+        <v>114</v>
       </c>
       <c r="C26" s="73">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D26" s="70"/>
       <c r="E26" s="70"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="71" t="s">
-        <v>114</v>
+        <v>143</v>
       </c>
       <c r="C27" s="73">
-        <v>0.5</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D27" s="70"/>
       <c r="E27" s="70"/>
@@ -50910,7 +50898,8 @@
         <v>115</v>
       </c>
       <c r="C28" s="73">
-        <v>2</v>
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D28" s="70"/>
       <c r="E28" s="70"/>
@@ -50920,7 +50909,8 @@
         <v>116</v>
       </c>
       <c r="C29" s="73">
-        <v>3</v>
+        <f>2/12</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D29" s="70"/>
       <c r="E29" s="70"/>
@@ -50930,130 +50920,128 @@
         <v>117</v>
       </c>
       <c r="C30" s="73">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D30" s="70"/>
       <c r="E30" s="70"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="71" t="s">
-        <v>147</v>
+        <v>118</v>
       </c>
       <c r="C31" s="73">
-        <v>3.5000000000000003E-2</v>
+        <v>0.9</v>
       </c>
       <c r="D31" s="70"/>
       <c r="E31" s="70"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="71" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C32" s="73">
-        <f>1/12</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.6</v>
       </c>
       <c r="D32" s="70"/>
       <c r="E32" s="70"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="71" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C33" s="73">
-        <f>2/12</f>
-        <v>0.16666666666666666</v>
+        <v>0.4</v>
       </c>
       <c r="D33" s="70"/>
       <c r="E33" s="70"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="71" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C34" s="73">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="D34" s="70"/>
       <c r="E34" s="70"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="71" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C35" s="73">
-        <v>0.9</v>
+        <v>4</v>
       </c>
       <c r="D35" s="70"/>
       <c r="E35" s="70"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="71" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C36" s="73">
-        <v>0.6</v>
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="D36" s="70"/>
       <c r="E36" s="70"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="71" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C37" s="73">
-        <v>0.4</v>
+        <v>1950</v>
       </c>
       <c r="D37" s="70"/>
       <c r="E37" s="70"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="71" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C38" s="73">
-        <v>0.25</v>
+        <v>2050</v>
       </c>
       <c r="D38" s="70"/>
       <c r="E38" s="70"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="71" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C39" s="73">
-        <v>4</v>
+        <v>1940</v>
       </c>
       <c r="D39" s="70"/>
       <c r="E39" s="70"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="71" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="C40" s="73">
-        <f>1/15</f>
-        <v>6.6666666666666666E-2</v>
+        <v>1990</v>
       </c>
       <c r="D40" s="70"/>
       <c r="E40" s="70"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="71" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C41" s="73">
-        <v>1950</v>
+        <v>2010</v>
       </c>
       <c r="D41" s="70"/>
       <c r="E41" s="70"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="71" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C42" s="73">
-        <v>2050</v>
+        <v>0</v>
       </c>
       <c r="D42" s="70"/>
       <c r="E42" s="70"/>
@@ -51063,7 +51051,7 @@
         <v>129</v>
       </c>
       <c r="C43" s="73">
-        <v>1940</v>
+        <v>0.85</v>
       </c>
       <c r="D43" s="70"/>
       <c r="E43" s="70"/>
@@ -51073,215 +51061,215 @@
         <v>131</v>
       </c>
       <c r="C44" s="73">
-        <v>1990</v>
+        <v>0.6</v>
       </c>
       <c r="D44" s="70"/>
       <c r="E44" s="70"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C45" s="73">
-        <v>2010</v>
+        <v>0.4</v>
       </c>
       <c r="D45" s="70"/>
       <c r="E45" s="70"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="71" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
       <c r="C46" s="73">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D46" s="70"/>
       <c r="E46" s="70"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="71" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C47" s="73">
-        <v>0.85</v>
+        <v>2</v>
       </c>
       <c r="D47" s="70"/>
       <c r="E47" s="70"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C48" s="73">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="D48" s="70"/>
       <c r="E48" s="70"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="71" t="s">
-        <v>135</v>
-      </c>
-      <c r="C49" s="73">
-        <v>0.4</v>
-      </c>
-      <c r="D49" s="70"/>
-      <c r="E49" s="70"/>
+      <c r="A49" s="5"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="71" t="s">
-        <v>148</v>
-      </c>
-      <c r="C50" s="73">
-        <v>0.4</v>
-      </c>
-      <c r="D50" s="70"/>
-      <c r="E50" s="70"/>
+      <c r="A50" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="71" t="s">
-        <v>149</v>
-      </c>
-      <c r="C51" s="73">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D51" s="70"/>
-      <c r="E51" s="70"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="71" t="s">
-        <v>136</v>
-      </c>
-      <c r="C52" s="73">
-        <v>0.25</v>
-      </c>
-      <c r="D52" s="70"/>
-      <c r="E52" s="70"/>
+        <v>99</v>
+      </c>
+      <c r="C52" s="72">
+        <v>20000000</v>
+      </c>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
+      <c r="B53" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="4">
+        <v>0</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B54" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" s="4">
+        <v>0</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B55" s="71" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" s="4">
+        <v>3</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="C56" s="72">
-        <v>20000000</v>
+      <c r="B56" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B57" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" s="4">
-        <v>0</v>
-      </c>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C58" s="4">
-        <v>0</v>
-      </c>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="8" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B59" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C59" s="4">
-        <v>3</v>
-      </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
+      <c r="C59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="4">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C60" s="9">
+        <v>0.2</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
     </row>
-    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>9</v>
-      </c>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C62" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C63" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B63" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C63" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C64" s="9">
-        <v>0.2</v>
+        <v>14</v>
+      </c>
+      <c r="C64" s="6">
+        <v>0.4</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C65" s="6">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C66" s="6">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C67" s="6">
         <v>0.5</v>
@@ -51289,48 +51277,8 @@
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B68" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C68" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
-    </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B69" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C69" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
-    </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B70" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C70" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-    </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B71" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C71" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-    </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="2">
+  <dataValidations count="2">
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Crude birth rate" prompt="Imports directly from world_bank_crude_birth_rates spreadsheet" sqref="C3:E3">
       <formula1>0</formula1>
       <formula2>0.2</formula2>

</xml_diff>

<commit_message>
Set fixed proportions by organ
Set proportions of patients progressing by organ status according to the
proportion of notifications in the GTB report
</commit_message>
<xml_diff>
--- a/autumn/xls/TB_generalepi_macro_constants.xlsx
+++ b/autumn/xls/TB_generalepi_macro_constants.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="143">
   <si>
     <t>best</t>
   </si>
@@ -322,15 +322,6 @@
   </si>
   <si>
     <t>susceptible_fully</t>
-  </si>
-  <si>
-    <t>epi_proportion_cases_smearpos</t>
-  </si>
-  <si>
-    <t>epi_proportion_cases_smearneg</t>
-  </si>
-  <si>
-    <t>epi_proportion_cases_extrapul</t>
   </si>
   <si>
     <t>tb_n_contact</t>
@@ -3225,10 +3216,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3243,10 +3234,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3264,184 +3255,181 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="71" t="s">
-        <v>100</v>
+        <v>129</v>
       </c>
       <c r="C3" s="73">
-        <f>(92991+6277)/243379</f>
-        <v>0.40787413868904054</v>
+        <v>0.24</v>
       </c>
       <c r="D3" s="70"/>
       <c r="E3" s="70"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="71" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C4" s="73">
-        <f>139950/243379</f>
-        <v>0.57502906988688429</v>
+        <v>14</v>
       </c>
       <c r="D4" s="70"/>
       <c r="E4" s="70"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="71" t="s">
-        <v>102</v>
+        <v>130</v>
       </c>
       <c r="C5" s="73">
-        <f>4161/243379</f>
-        <v>1.7096791424075209E-2</v>
+        <v>0.12</v>
       </c>
       <c r="D5" s="70"/>
       <c r="E5" s="70"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C6" s="73">
-        <v>0.24</v>
+        <v>0.4</v>
       </c>
       <c r="D6" s="70"/>
       <c r="E6" s="70"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="71" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C7" s="73">
-        <v>14</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="D7" s="70"/>
       <c r="E7" s="70"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="71" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C8" s="73">
-        <v>0.12</v>
+        <v>0.7</v>
       </c>
       <c r="D8" s="70"/>
       <c r="E8" s="70"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="71" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="73">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="D9" s="70"/>
       <c r="E9" s="70"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="71" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="73">
-        <v>7.0000000000000001E-3</v>
+        <v>0.4</v>
       </c>
       <c r="D10" s="70"/>
       <c r="E10" s="70"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="71" t="s">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="C11" s="73">
-        <v>0.7</v>
+        <v>3</v>
       </c>
       <c r="D11" s="70"/>
       <c r="E11" s="70"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="71" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C12" s="73">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="D12" s="70"/>
       <c r="E12" s="70"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="71" t="s">
-        <v>105</v>
+        <v>135</v>
       </c>
       <c r="C13" s="73">
-        <v>0.4</v>
+        <v>0.88</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="71" t="s">
-        <v>106</v>
+        <v>136</v>
       </c>
       <c r="C14" s="73">
-        <v>3</v>
+        <f>1-C13</f>
+        <v>0.12</v>
       </c>
       <c r="D14" s="70"/>
       <c r="E14" s="70"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="71" t="s">
-        <v>137</v>
+        <v>104</v>
       </c>
       <c r="C15" s="73">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="71" t="s">
-        <v>138</v>
+        <v>105</v>
       </c>
       <c r="C16" s="73">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="70"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="71" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C17" s="73">
-        <f>1-C16</f>
-        <v>0.12</v>
+        <v>26</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="71" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C18" s="73">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="D18" s="70"/>
       <c r="E18" s="70"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="71" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" s="73">
-        <v>0.9</v>
+        <v>2</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="70"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="71" t="s">
-        <v>140</v>
+        <v>108</v>
       </c>
       <c r="C20" s="73">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D20" s="70"/>
       <c r="E20" s="70"/>
@@ -3451,47 +3439,49 @@
         <v>109</v>
       </c>
       <c r="C21" s="73">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="D21" s="70"/>
       <c r="E21" s="70"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="71" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="C22" s="73">
-        <v>2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D22" s="70"/>
       <c r="E22" s="70"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="71" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C23" s="73">
-        <v>3</v>
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D23" s="70"/>
       <c r="E23" s="70"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="71" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C24" s="73">
-        <v>3</v>
+        <f>2/12</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D24" s="70"/>
       <c r="E24" s="70"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="71" t="s">
-        <v>141</v>
+        <v>112</v>
       </c>
       <c r="C25" s="73">
-        <v>3.5000000000000003E-2</v>
+        <v>2</v>
       </c>
       <c r="D25" s="70"/>
       <c r="E25" s="70"/>
@@ -3501,8 +3491,7 @@
         <v>113</v>
       </c>
       <c r="C26" s="73">
-        <f>1/12</f>
-        <v>8.3333333333333329E-2</v>
+        <v>0.9</v>
       </c>
       <c r="D26" s="70"/>
       <c r="E26" s="70"/>
@@ -3512,8 +3501,7 @@
         <v>114</v>
       </c>
       <c r="C27" s="73">
-        <f>2/12</f>
-        <v>0.16666666666666666</v>
+        <v>0.6</v>
       </c>
       <c r="D27" s="70"/>
       <c r="E27" s="70"/>
@@ -3523,7 +3511,7 @@
         <v>115</v>
       </c>
       <c r="C28" s="73">
-        <v>2</v>
+        <v>0.4</v>
       </c>
       <c r="D28" s="70"/>
       <c r="E28" s="70"/>
@@ -3533,7 +3521,7 @@
         <v>116</v>
       </c>
       <c r="C29" s="73">
-        <v>0.9</v>
+        <v>0.25</v>
       </c>
       <c r="D29" s="70"/>
       <c r="E29" s="70"/>
@@ -3543,7 +3531,7 @@
         <v>117</v>
       </c>
       <c r="C30" s="73">
-        <v>0.6</v>
+        <v>4</v>
       </c>
       <c r="D30" s="70"/>
       <c r="E30" s="70"/>
@@ -3553,7 +3541,8 @@
         <v>118</v>
       </c>
       <c r="C31" s="73">
-        <v>0.4</v>
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="D31" s="70"/>
       <c r="E31" s="70"/>
@@ -3563,7 +3552,7 @@
         <v>119</v>
       </c>
       <c r="C32" s="73">
-        <v>0.25</v>
+        <v>1950</v>
       </c>
       <c r="D32" s="70"/>
       <c r="E32" s="70"/>
@@ -3573,7 +3562,7 @@
         <v>120</v>
       </c>
       <c r="C33" s="73">
-        <v>4</v>
+        <v>2050</v>
       </c>
       <c r="D33" s="70"/>
       <c r="E33" s="70"/>
@@ -3583,170 +3572,169 @@
         <v>121</v>
       </c>
       <c r="C34" s="73">
-        <f>1/15</f>
-        <v>6.6666666666666666E-2</v>
+        <v>1940</v>
       </c>
       <c r="D34" s="70"/>
       <c r="E34" s="70"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="71" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C35" s="73">
-        <v>1950</v>
+        <v>1990</v>
       </c>
       <c r="D35" s="70"/>
       <c r="E35" s="70"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="71" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C36" s="73">
-        <v>2050</v>
+        <v>2010</v>
       </c>
       <c r="D36" s="70"/>
       <c r="E36" s="70"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="71" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C37" s="73">
-        <v>1940</v>
+        <v>0</v>
       </c>
       <c r="D37" s="70"/>
       <c r="E37" s="70"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="71" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C38" s="73">
-        <v>1990</v>
+        <v>0.85</v>
       </c>
       <c r="D38" s="70"/>
       <c r="E38" s="70"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="71" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C39" s="73">
-        <v>2010</v>
+        <v>0.6</v>
       </c>
       <c r="D39" s="70"/>
       <c r="E39" s="70"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="71" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C40" s="73">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="D40" s="70"/>
       <c r="E40" s="70"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="71" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C41" s="73">
-        <v>0.85</v>
+        <v>0.4</v>
       </c>
       <c r="D41" s="70"/>
       <c r="E41" s="70"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B42" s="71" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
       <c r="C42" s="73">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="D42" s="70"/>
       <c r="E42" s="70"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B43" s="71" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C43" s="73">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D43" s="70"/>
       <c r="E43" s="70"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="71" t="s">
-        <v>142</v>
-      </c>
-      <c r="C44" s="73">
-        <v>0.4</v>
-      </c>
-      <c r="D44" s="70"/>
-      <c r="E44" s="70"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="71" t="s">
-        <v>143</v>
-      </c>
-      <c r="C45" s="73">
+      <c r="A45" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D45" s="70"/>
-      <c r="E45" s="70"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="71" t="s">
-        <v>131</v>
-      </c>
-      <c r="C46" s="73">
-        <v>0.25</v>
-      </c>
-      <c r="D46" s="70"/>
-      <c r="E46" s="70"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
+      <c r="B47" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="72">
+        <v>20000000</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B48" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C48" s="4">
+        <v>0</v>
+      </c>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="3" t="s">
+      <c r="B49" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" s="4">
         <v>0</v>
       </c>
-      <c r="D49" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="C50" s="72">
-        <v>20000000</v>
+        <v>7</v>
+      </c>
+      <c r="C50" s="4">
+        <v>3</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C51" s="4">
         <v>0</v>
@@ -3754,131 +3742,101 @@
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C52" s="4">
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C54" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C53" s="4">
-        <v>3</v>
-      </c>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B54" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="4">
-        <v>0</v>
-      </c>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
-    </row>
-    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="D54" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C57" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C58" s="9">
-        <v>0.2</v>
+      <c r="B58" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="6">
+        <v>0.5</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C59" s="6">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C60" s="6">
-        <v>0.9</v>
+        <v>0.1</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="7" t="s">
-        <v>13</v>
+      <c r="B61" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C61" s="6">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="1" t="s">
-        <v>14</v>
+      <c r="B62" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C62" s="6">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B63" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C63" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B64" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C64" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-    </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B65" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C65" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Reducing constants for parameter reader
Trying to whittle down the number of constants needed for the parameter
spreadhseet reader - to make the next step a bit simpler
</commit_message>
<xml_diff>
--- a/autumn/xls/TB_generalepi_macro_constants.xlsx
+++ b/autumn/xls/TB_generalepi_macro_constants.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="542" uniqueCount="141">
   <si>
     <t>best</t>
   </si>
@@ -427,12 +427,6 @@
   </si>
   <si>
     <t>tb_multiplier_bcg_protection</t>
-  </si>
-  <si>
-    <t>program_prop_vac</t>
-  </si>
-  <si>
-    <t>program_prop_unvac</t>
   </si>
   <si>
     <t>program_rate_start_treatment</t>
@@ -3216,10 +3210,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:E62"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3234,10 +3228,10 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3355,366 +3349,365 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="71" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="C13" s="73">
-        <v>0.88</v>
+        <v>0.8</v>
       </c>
       <c r="D13" s="70"/>
       <c r="E13" s="70"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="71" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
       <c r="C14" s="73">
-        <f>1-C13</f>
-        <v>0.12</v>
+        <v>0.9</v>
       </c>
       <c r="D14" s="70"/>
       <c r="E14" s="70"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="71" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="C15" s="73">
-        <v>0.8</v>
+        <v>26</v>
       </c>
       <c r="D15" s="70"/>
       <c r="E15" s="70"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="71" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C16" s="73">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="70"/>
       <c r="E16" s="70"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="71" t="s">
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="C17" s="73">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D17" s="70"/>
       <c r="E17" s="70"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="71" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C18" s="73">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="D18" s="70"/>
       <c r="E18" s="70"/>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="71" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C19" s="73">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D19" s="70"/>
       <c r="E19" s="70"/>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="71" t="s">
-        <v>108</v>
+        <v>136</v>
       </c>
       <c r="C20" s="73">
-        <v>3</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="D20" s="70"/>
       <c r="E20" s="70"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="71" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C21" s="73">
-        <v>3</v>
+        <f>1/12</f>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D21" s="70"/>
       <c r="E21" s="70"/>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="71" t="s">
-        <v>138</v>
+        <v>111</v>
       </c>
       <c r="C22" s="73">
-        <v>3.5000000000000003E-2</v>
+        <f>2/12</f>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D22" s="70"/>
       <c r="E22" s="70"/>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="71" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C23" s="73">
-        <f>1/12</f>
-        <v>8.3333333333333329E-2</v>
+        <v>2</v>
       </c>
       <c r="D23" s="70"/>
       <c r="E23" s="70"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="71" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C24" s="73">
-        <f>2/12</f>
-        <v>0.16666666666666666</v>
+        <v>0.9</v>
       </c>
       <c r="D24" s="70"/>
       <c r="E24" s="70"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="71" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C25" s="73">
-        <v>2</v>
+        <v>0.6</v>
       </c>
       <c r="D25" s="70"/>
       <c r="E25" s="70"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="71" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C26" s="73">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D26" s="70"/>
       <c r="E26" s="70"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="71" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C27" s="73">
-        <v>0.6</v>
+        <v>0.25</v>
       </c>
       <c r="D27" s="70"/>
       <c r="E27" s="70"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B28" s="71" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C28" s="73">
-        <v>0.4</v>
+        <v>4</v>
       </c>
       <c r="D28" s="70"/>
       <c r="E28" s="70"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="71" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C29" s="73">
-        <v>0.25</v>
+        <f>1/15</f>
+        <v>6.6666666666666666E-2</v>
       </c>
       <c r="D29" s="70"/>
       <c r="E29" s="70"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="71" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C30" s="73">
-        <v>4</v>
+        <v>1950</v>
       </c>
       <c r="D30" s="70"/>
       <c r="E30" s="70"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="71" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C31" s="73">
-        <f>1/15</f>
-        <v>6.6666666666666666E-2</v>
+        <v>2050</v>
       </c>
       <c r="D31" s="70"/>
       <c r="E31" s="70"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="71" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C32" s="73">
-        <v>1950</v>
+        <v>1940</v>
       </c>
       <c r="D32" s="70"/>
       <c r="E32" s="70"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" s="71" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C33" s="73">
-        <v>2050</v>
+        <v>1990</v>
       </c>
       <c r="D33" s="70"/>
       <c r="E33" s="70"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B34" s="71" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C34" s="73">
-        <v>1940</v>
+        <v>2010</v>
       </c>
       <c r="D34" s="70"/>
       <c r="E34" s="70"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B35" s="71" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C35" s="73">
-        <v>1990</v>
+        <v>0</v>
       </c>
       <c r="D35" s="70"/>
       <c r="E35" s="70"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="71" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C36" s="73">
-        <v>2010</v>
+        <v>0.85</v>
       </c>
       <c r="D36" s="70"/>
       <c r="E36" s="70"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="71" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="C37" s="73">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="D37" s="70"/>
       <c r="E37" s="70"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="71" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C38" s="73">
-        <v>0.85</v>
+        <v>0.4</v>
       </c>
       <c r="D38" s="70"/>
       <c r="E38" s="70"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="71" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C39" s="73">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="D39" s="70"/>
       <c r="E39" s="70"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" s="71" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C40" s="73">
-        <v>0.4</v>
+        <v>2</v>
       </c>
       <c r="D40" s="70"/>
       <c r="E40" s="70"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" s="71" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
       <c r="C41" s="73">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="D41" s="70"/>
       <c r="E41" s="70"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="71" t="s">
-        <v>140</v>
-      </c>
-      <c r="C42" s="73">
+      <c r="A42" s="5"/>
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D42" s="70"/>
-      <c r="E42" s="70"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="71" t="s">
-        <v>128</v>
-      </c>
-      <c r="C43" s="73">
-        <v>0.25</v>
-      </c>
-      <c r="D43" s="70"/>
-      <c r="E43" s="70"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="5"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="B45" s="71" t="s">
+        <v>99</v>
+      </c>
+      <c r="C45" s="72">
+        <v>20000000</v>
+      </c>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="3" t="s">
+      <c r="B46" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" s="4">
         <v>0</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="71" t="s">
-        <v>99</v>
-      </c>
-      <c r="C47" s="72">
-        <v>20000000</v>
+      <c r="B47" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" s="4">
+        <v>0</v>
       </c>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B48" s="1" t="s">
-        <v>5</v>
+      <c r="B48" s="71" t="s">
+        <v>7</v>
       </c>
       <c r="C48" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D48" s="4"/>
       <c r="E48" s="4"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C49" s="4">
         <v>0</v>
@@ -3722,121 +3715,101 @@
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="71" t="s">
-        <v>7</v>
-      </c>
-      <c r="C50" s="4">
-        <v>3</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C51" s="4">
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C52" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-    </row>
-    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="8" t="s">
-        <v>9</v>
-      </c>
+      <c r="D52" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C54" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E54" s="3" t="s">
-        <v>2</v>
-      </c>
+      <c r="B54" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="6">
+        <v>0.6</v>
+      </c>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C55" s="9">
-        <v>0.2</v>
+        <v>12</v>
+      </c>
+      <c r="C55" s="6">
+        <v>0.9</v>
       </c>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="1" t="s">
-        <v>11</v>
+      <c r="B56" s="7" t="s">
+        <v>13</v>
       </c>
       <c r="C56" s="6">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C57" s="6">
-        <v>0.9</v>
+        <v>0.4</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B58" s="7" t="s">
-        <v>13</v>
+      <c r="B58" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C58" s="6">
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C59" s="6">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B60" s="1" t="s">
-        <v>15</v>
+      <c r="B60" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="C60" s="6">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B61" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C61" s="6">
-        <v>0.3</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B62" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>